<commit_message>
update departmentid for OUTSOURCE
</commit_message>
<xml_diff>
--- a/Excels/Department2.xlsx
+++ b/Excels/Department2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\workspace\SurplusMigrator\SurplusMigrator-ExternalSource\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A08AE3C-5D26-4109-9C6A-E85F08C6C5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5027758-3416-4856-A8AF-4AFF8F41B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="3150" windowWidth="21600" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="3495" windowWidth="21600" windowHeight="11415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$594</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -5468,7 +5468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F594"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
@@ -16304,10 +16304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16316,7 +16316,7 @@
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1642</v>
       </c>
@@ -16329,8 +16329,12 @@
       <c r="D1" t="s">
         <v>1682</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="str">
+        <f>IFERROR(INDEX($D$2:$D$10, MATCH(0, COUNTIF($D$1:D1, $D$2:$D$10), 0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -16338,7 +16342,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -16352,7 +16356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -16366,7 +16370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -16380,7 +16384,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -16394,7 +16398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1008</v>
       </c>
@@ -16408,7 +16412,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1009</v>
       </c>
@@ -16422,7 +16426,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1010</v>
       </c>
@@ -16436,7 +16440,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1012</v>
       </c>
@@ -16450,7 +16454,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1015</v>
       </c>
@@ -16464,7 +16468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1027</v>
       </c>
@@ -16478,7 +16482,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1035</v>
       </c>
@@ -16492,7 +16496,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1500</v>
       </c>
@@ -16510,7 +16514,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1502</v>
       </c>
@@ -16528,7 +16532,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1510</v>
       </c>

</xml_diff>